<commit_message>
Throw error when lecturer is unavailable too many days
</commit_message>
<xml_diff>
--- a/system_storage/history/programme/BCS-September-2024 S1.xlsx
+++ b/system_storage/history/programme/BCS-September-2024 S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Day / Time</t>
   </si>
@@ -85,14 +85,19 @@
 JC1</t>
   </si>
   <si>
-    <t>ENG1044-G3-Tutorial
-(Herrick Yeap Han Lin)
-UE2-16</t>
-  </si>
-  <si>
-    <t>MTH1114-G5-Tutorial
+    <t>MTH1114-G1-Tutorial
 (Jaya Krishna)
-UE2-17</t>
+UC3-3</t>
+  </si>
+  <si>
+    <t>MTH1114-G2-Tutorial
+(Jaya Krishna)
+UC3-3</t>
+  </si>
+  <si>
+    <t>MTH1114-G3-Tutorial
+(Jaya Krishna)
+UC3-3</t>
   </si>
   <si>
     <t>Monday</t>
@@ -103,32 +108,32 @@
 JC1</t>
   </si>
   <si>
-    <t>MTH1114-G4-Tutorial
-(Jaya Krishna)
-UE2-17</t>
+    <t>CSC1202-G4-Practical
+(Chew Moi Tin)
+UE2-16</t>
+  </si>
+  <si>
+    <t>ENG1044-G1-Tutorial
+(Herrick Yeap Han Lin)
+UC3-3</t>
+  </si>
+  <si>
+    <t>ENG1044-G2-Tutorial
+(Herrick Yeap Han Lin)
+UC3-4</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>ENG1044-G4-Tutorial
+(Herrick Yeap Han Lin)
+UC3-4</t>
   </si>
   <si>
     <t>CSC1202-G1-Practical
 (Chew Moi Tin)
 UE2-16</t>
-  </si>
-  <si>
-    <t>MTH1114-G6-Tutorial
-(Jaya Krishna)
-UE2-17</t>
-  </si>
-  <si>
-    <t>CSC1202-G2-Practical
-(Chew Moi Tin)
-UE2-16</t>
-  </si>
-  <si>
-    <t>CSC1202-G3-Practical
-(Chew Moi Tin)
-UE2-16</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
   </si>
   <si>
     <t>MTH1114-G1-Lecture
@@ -136,26 +141,16 @@
 JC1</t>
   </si>
   <si>
-    <t>CSC1202-G4-Practical
+    <t>CSC1202-G2-Practical
 (Chew Moi Tin)
 UE2-16</t>
   </si>
   <si>
-    <t>CSC1202-G5-Practical
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>CSC1202-G3-Practical
 (Chew Moi Tin)
-UE2-16</t>
-  </si>
-  <si>
-    <t>CSC1202-G6-Practical
-(Chew Moi Tin)
-UE2-16</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>CSC1024-G6-Practical
-(Tan Kai Wei)
 UE2-16</t>
   </si>
   <si>
@@ -167,14 +162,9 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>ENG1044-G5-Tutorial
-(Herrick Yeap Han Lin)
-UC3-3</t>
-  </si>
-  <si>
-    <t>MTH1114-G1-Tutorial
+    <t>MTH1114-G4-Tutorial
 (Jaya Krishna)
-UE2-17</t>
+UC3-4</t>
   </si>
   <si>
     <t>CSC1024-G1-Practical
@@ -182,16 +172,16 @@
 UE2-16</t>
   </si>
   <si>
+    <t>ENG1044-G3-Tutorial
+(Herrick Yeap Han Lin)
+UC3-4</t>
+  </si>
+  <si>
     <t>CSC1024-G2-Practical
 (Tan Kai Wei)
 UE2-16</t>
   </si>
   <si>
-    <t>ENG1044-G6-Tutorial
-(Herrick Yeap Han Lin)
-UC3-3</t>
-  </si>
-  <si>
     <t>CSC1024-G3-Practical
 (Farrukh Hassan)
 UE2-16</t>
@@ -202,28 +192,13 @@
 UE2-16</t>
   </si>
   <si>
-    <t>MTH1114-G2-Tutorial
-(Jaya Krishna)
-UE2-17</t>
-  </si>
-  <si>
-    <t>ENG1044-G4-Tutorial
-(Herrick Yeap Han Lin)
-UC3-3</t>
-  </si>
-  <si>
-    <t>CSC1024-G5-Practical
-(Farrukh Hassan)
-UE2-16</t>
-  </si>
-  <si>
     <t>Friday</t>
   </si>
   <si>
     <t>Timetable Fitness Score:</t>
   </si>
   <si>
-    <t>99.03%</t>
+    <t>98.9%</t>
   </si>
 </sst>
 </file>
@@ -367,13 +342,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.59375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="9.8984375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="5.4921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="5.4921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="5.4921875" customWidth="true" bestFit="true"/>
@@ -467,150 +442,125 @@
     </row>
     <row r="2" ht="62.4" customHeight="true">
       <c r="A2" t="s" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s" s="3">
         <v>22</v>
       </c>
-      <c r="J2" t="s" s="4">
+      <c r="F2" t="s" s="4">
         <v>23</v>
       </c>
+      <c r="K2" t="s" s="4">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" ht="62.4" customHeight="true">
+      <c r="A3" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s" s="5">
+        <v>28</v>
+      </c>
       <c r="J3" t="s" s="4">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="O3" t="s" s="4">
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="62.4" customHeight="true">
       <c r="A4" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="B4" t="s" s="3">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s" s="4">
-        <v>27</v>
-      </c>
-      <c r="J4" t="s" s="4">
-        <v>29</v>
-      </c>
-      <c r="P4" t="s" s="5">
-        <v>31</v>
+      <c r="F4" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s" s="5">
+        <v>35</v>
       </c>
     </row>
     <row r="5" ht="62.4" customHeight="true">
-      <c r="F5" t="s" s="5">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s" s="5">
-        <v>30</v>
+      <c r="B5" t="s" s="5">
+        <v>33</v>
       </c>
     </row>
     <row r="6" ht="62.4" customHeight="true">
       <c r="A6" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="B6" t="s" s="3">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s" s="5">
-        <v>34</v>
-      </c>
-      <c r="K6" t="s" s="5">
-        <v>35</v>
-      </c>
-      <c r="P6" t="s" s="5">
-        <v>36</v>
+      <c r="J6" t="s" s="3">
+        <v>38</v>
       </c>
     </row>
     <row r="7" ht="62.4" customHeight="true">
       <c r="A7" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="B7" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s" s="3">
-        <v>39</v>
+      <c r="F7" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="J7" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="N7" t="s" s="5">
+        <v>45</v>
       </c>
     </row>
     <row r="8" ht="62.4" customHeight="true">
-      <c r="A8" t="s" s="1">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" t="s" s="5">
         <v>41</v>
       </c>
       <c r="F8" t="s" s="5">
-        <v>44</v>
-      </c>
-      <c r="J8" t="s" s="5">
-        <v>46</v>
-      </c>
-      <c r="N8" t="s" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="R8" t="s" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" ht="62.4" customHeight="true">
-      <c r="B9" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s" s="4">
-        <v>45</v>
-      </c>
-      <c r="Q9" t="s" s="4">
+      <c r="B10" t="s" s="6">
         <v>48</v>
       </c>
     </row>
-    <row r="10" ht="62.4" customHeight="true">
-      <c r="B10" t="s" s="5">
-        <v>43</v>
-      </c>
-      <c r="Q10" t="s" s="4">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s" s="6">
-        <v>53</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="22">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
     <mergeCell ref="J3:M3"/>
-    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="O3:R3"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="F4:I4"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="N4:Q4"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="J6:M6"/>
     <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="F7:I7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
     <mergeCell ref="F8:I8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="Q9:T9"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="R8:U8"/>
-    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>